<commit_message>
made individual D3 charts for number of crashes, number of injuries and fatalities
</commit_message>
<xml_diff>
--- a/0425/second_draft.xlsx
+++ b/0425/second_draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1720" windowWidth="24800" windowHeight="11600" tabRatio="878" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24780" windowHeight="15600" tabRatio="878"/>
   </bookViews>
   <sheets>
     <sheet name="no_of_crashes" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="164">
   <si>
     <t>crashType</t>
   </si>
@@ -588,8 +588,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -601,11 +603,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,7 +642,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[4]Number of crashes'!$B$1</c:f>
+              <c:f>'[1]Number of crashes'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -649,48 +653,48 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'[4]Number of crashes'!$A$2:$A$12</c:f>
+              <c:f>'[1]Number of crashes'!$A$2:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>"05</c:v>
+                  <c:v>_x0003_"05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>"06</c:v>
+                  <c:v>_x0003_"06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>"07</c:v>
+                  <c:v>_x0003_"07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>"08</c:v>
+                  <c:v>_x0003_"08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>"09</c:v>
+                  <c:v>_x0003_"09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>"10</c:v>
+                  <c:v>_x0003_"10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>"11</c:v>
+                  <c:v>_x0003_"11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>"12</c:v>
+                  <c:v>_x0003_"12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>"13</c:v>
+                  <c:v>_x0003_"13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>"14</c:v>
+                  <c:v>_x0003_"14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>"15</c:v>
+                  <c:v>_x0003_"15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[4]Number of crashes'!$B$2:$B$12</c:f>
+              <c:f>'[1]Number of crashes'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -736,7 +740,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[4]Number of crashes'!$C$1</c:f>
+              <c:f>'[1]Number of crashes'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -747,48 +751,48 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'[4]Number of crashes'!$A$2:$A$12</c:f>
+              <c:f>'[1]Number of crashes'!$A$2:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>"05</c:v>
+                  <c:v>_x0003_"05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>"06</c:v>
+                  <c:v>_x0003_"06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>"07</c:v>
+                  <c:v>_x0003_"07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>"08</c:v>
+                  <c:v>_x0003_"08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>"09</c:v>
+                  <c:v>_x0003_"09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>"10</c:v>
+                  <c:v>_x0003_"10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>"11</c:v>
+                  <c:v>_x0003_"11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>"12</c:v>
+                  <c:v>_x0003_"12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>"13</c:v>
+                  <c:v>_x0003_"13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>"14</c:v>
+                  <c:v>_x0003_"14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>"15</c:v>
+                  <c:v>_x0003_"15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[4]Number of crashes'!$C$2:$C$12</c:f>
+              <c:f>'[1]Number of crashes'!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -834,7 +838,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[4]Number of crashes'!$D$1</c:f>
+              <c:f>'[1]Number of crashes'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -845,48 +849,48 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'[4]Number of crashes'!$A$2:$A$12</c:f>
+              <c:f>'[1]Number of crashes'!$A$2:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>"05</c:v>
+                  <c:v>_x0003_"05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>"06</c:v>
+                  <c:v>_x0003_"06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>"07</c:v>
+                  <c:v>_x0003_"07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>"08</c:v>
+                  <c:v>_x0003_"08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>"09</c:v>
+                  <c:v>_x0003_"09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>"10</c:v>
+                  <c:v>_x0003_"10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>"11</c:v>
+                  <c:v>_x0003_"11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>"12</c:v>
+                  <c:v>_x0003_"12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>"13</c:v>
+                  <c:v>_x0003_"13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>"14</c:v>
+                  <c:v>_x0003_"14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>"15</c:v>
+                  <c:v>_x0003_"15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[4]Number of crashes'!$D$2:$D$12</c:f>
+              <c:f>'[1]Number of crashes'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -902,11 +906,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2102639992"/>
-        <c:axId val="-2115884792"/>
+        <c:axId val="-2104760952"/>
+        <c:axId val="-2102787064"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2102639992"/>
+        <c:axId val="-2104760952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -915,7 +919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115884792"/>
+        <c:crossAx val="-2102787064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -923,7 +927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115884792"/>
+        <c:axId val="-2102787064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102639992"/>
+        <c:crossAx val="-2104760952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -971,7 +975,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1067,7 +1070,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1110,7 +1112,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[3]fixedobject!$B$1</c:f>
+              <c:f>[4]fixedobject!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1121,7 +1123,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>[3]fixedobject!$A$2:$A$30</c:f>
+              <c:f>[4]fixedobject!$A$2:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
@@ -1217,7 +1219,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[3]fixedobject!$B$2:$B$30</c:f>
+              <c:f>[4]fixedobject!$B$2:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -1356,7 +1358,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1370,7 +1371,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[4]number of fatalities'!$B$1</c:f>
+              <c:f>'[1]number of fatalities'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1384,48 +1385,48 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'[4]number of fatalities'!$A$2:$A$12</c:f>
+              <c:f>'[1]number of fatalities'!$A$2:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>"05</c:v>
+                  <c:v>_x0003_"05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>"06</c:v>
+                  <c:v>_x0003_"06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>"07</c:v>
+                  <c:v>_x0003_"07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>"08</c:v>
+                  <c:v>_x0003_"08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>"09</c:v>
+                  <c:v>_x0003_"09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>"10</c:v>
+                  <c:v>_x0003_"10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>"11</c:v>
+                  <c:v>_x0003_"11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>"12</c:v>
+                  <c:v>_x0003_"12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>"13</c:v>
+                  <c:v>_x0003_"13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>"14</c:v>
+                  <c:v>_x0003_"14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>"15</c:v>
+                  <c:v>_x0003_"15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[4]number of fatalities'!$B$2:$B$12</c:f>
+              <c:f>'[1]number of fatalities'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1477,11 +1478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2102036616"/>
-        <c:axId val="-2122122056"/>
+        <c:axId val="-2104544168"/>
+        <c:axId val="-2102251784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2102036616"/>
+        <c:axId val="-2104544168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1490,7 +1491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122122056"/>
+        <c:crossAx val="-2102251784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1498,7 +1499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122122056"/>
+        <c:axId val="-2102251784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,14 +1510,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102036616"/>
+        <c:crossAx val="-2104544168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1546,7 +1546,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1560,7 +1559,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[4]number of injuries'!$B$1</c:f>
+              <c:f>'[1]number of injuries'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1574,48 +1573,48 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'[4]number of injuries'!$A$2:$A$12</c:f>
+              <c:f>'[1]number of injuries'!$A$2:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>"05</c:v>
+                  <c:v>_x0003_"05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>"06</c:v>
+                  <c:v>_x0003_"06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>"07</c:v>
+                  <c:v>_x0003_"07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>"08</c:v>
+                  <c:v>_x0003_"08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>"09</c:v>
+                  <c:v>_x0003_"09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>"10</c:v>
+                  <c:v>_x0003_"10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>"11</c:v>
+                  <c:v>_x0003_"11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>"12</c:v>
+                  <c:v>_x0003_"12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>"13</c:v>
+                  <c:v>_x0003_"13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>"14</c:v>
+                  <c:v>_x0003_"14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>"15</c:v>
+                  <c:v>_x0003_"15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[4]number of injuries'!$B$2:$B$12</c:f>
+              <c:f>'[1]number of injuries'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1667,11 +1666,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103355624"/>
-        <c:axId val="-2103354216"/>
+        <c:axId val="-2102180968"/>
+        <c:axId val="-2128910248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2103355624"/>
+        <c:axId val="-2102180968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +1679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103354216"/>
+        <c:crossAx val="-2128910248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1688,7 +1687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103354216"/>
+        <c:axId val="-2128910248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,14 +1698,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103355624"/>
+        <c:crossAx val="-2102180968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1880,11 +1878,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2105514104"/>
-        <c:axId val="-2115382440"/>
+        <c:axId val="-2103268872"/>
+        <c:axId val="-2105261848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2105514104"/>
+        <c:axId val="-2103268872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1894,7 +1892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115382440"/>
+        <c:crossAx val="-2105261848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1902,7 +1900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115382440"/>
+        <c:axId val="-2105261848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1913,14 +1911,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105514104"/>
+        <c:crossAx val="-2103268872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2033,11 +2030,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2128333400"/>
-        <c:axId val="-2128389880"/>
+        <c:axId val="-2102238168"/>
+        <c:axId val="-2102047288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128333400"/>
+        <c:axId val="-2102238168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2046,7 +2043,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128389880"/>
+        <c:crossAx val="-2102047288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2054,7 +2051,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128389880"/>
+        <c:axId val="-2102047288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2065,14 +2062,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128333400"/>
+        <c:crossAx val="-2102238168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2102,7 +2098,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2117,7 +2112,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]fatal_crashtype!$B$1</c:f>
+              <c:f>[3]fatal_crashtype!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2129,7 +2124,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>[1]fatal_crashtype!$A$2:$A$8</c:f>
+              <c:f>[3]fatal_crashtype!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2159,7 +2154,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]fatal_crashtype!$B$2:$B$8</c:f>
+              <c:f>[3]fatal_crashtype!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2197,11 +2192,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2127314760"/>
-        <c:axId val="-2120054968"/>
+        <c:axId val="-2104834984"/>
+        <c:axId val="-2102795288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127314760"/>
+        <c:axId val="-2104834984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2205,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120054968"/>
+        <c:crossAx val="-2102795288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2218,7 +2213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120054968"/>
+        <c:axId val="-2102795288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,14 +2224,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127314760"/>
+        <c:crossAx val="-2104834984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2266,7 +2260,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2414,11 +2407,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2118892744"/>
-        <c:axId val="-2116662536"/>
+        <c:axId val="-2128639176"/>
+        <c:axId val="-2101778920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2118892744"/>
+        <c:axId val="-2128639176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2427,7 +2420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116662536"/>
+        <c:crossAx val="-2101778920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2435,7 +2428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2116662536"/>
+        <c:axId val="-2101778920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2446,14 +2439,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118892744"/>
+        <c:crossAx val="-2128639176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2597,11 +2589,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2115842696"/>
-        <c:axId val="-2115841288"/>
+        <c:axId val="-2104556296"/>
+        <c:axId val="-2104553288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2115842696"/>
+        <c:axId val="-2104556296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2610,7 +2602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115841288"/>
+        <c:crossAx val="-2104553288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2618,7 +2610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115841288"/>
+        <c:axId val="-2104553288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2629,14 +2621,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115842696"/>
+        <c:crossAx val="-2104556296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2752,11 +2743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105928888"/>
-        <c:axId val="-2117167448"/>
+        <c:axId val="-2102270616"/>
+        <c:axId val="-2102267672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105928888"/>
+        <c:axId val="-2102270616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,7 +2757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117167448"/>
+        <c:crossAx val="-2102267672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2774,7 +2765,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117167448"/>
+        <c:axId val="-2102267672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2785,14 +2776,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105928888"/>
+        <c:crossAx val="-2102270616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3206,6 +3196,747 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Number of crashes"/>
+      <sheetName val="number of fatalities"/>
+      <sheetName val="number of injuries"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>no of 911 calls regarding collisions</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>no of STARS report</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>no of self-report</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>"05</v>
+          </cell>
+          <cell r="B2">
+            <v>6095</v>
+          </cell>
+          <cell r="C2">
+            <v>3469</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>"06</v>
+          </cell>
+          <cell r="B3">
+            <v>6009</v>
+          </cell>
+          <cell r="C3">
+            <v>3462</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>"07</v>
+          </cell>
+          <cell r="B4">
+            <v>6194</v>
+          </cell>
+          <cell r="C4">
+            <v>3158</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>"08</v>
+          </cell>
+          <cell r="B5">
+            <v>5659</v>
+          </cell>
+          <cell r="C5">
+            <v>2906</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>"09</v>
+          </cell>
+          <cell r="B6">
+            <v>5364</v>
+          </cell>
+          <cell r="C6">
+            <v>2780</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>"10</v>
+          </cell>
+          <cell r="B7">
+            <v>5738</v>
+          </cell>
+          <cell r="C7">
+            <v>1847</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>"11</v>
+          </cell>
+          <cell r="B8">
+            <v>5492</v>
+          </cell>
+          <cell r="C8">
+            <v>1585</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>"12</v>
+          </cell>
+          <cell r="B9">
+            <v>5401</v>
+          </cell>
+          <cell r="C9">
+            <v>1556</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>"13</v>
+          </cell>
+          <cell r="B10">
+            <v>5613</v>
+          </cell>
+          <cell r="C10">
+            <v>1561</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>"14</v>
+          </cell>
+          <cell r="B11">
+            <v>5838</v>
+          </cell>
+          <cell r="C11">
+            <v>1524</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>"15</v>
+          </cell>
+          <cell r="B12">
+            <v>5887</v>
+          </cell>
+          <cell r="C12">
+            <v>1380</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Number of fatalities</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>"05</v>
+          </cell>
+          <cell r="B2">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>"06</v>
+          </cell>
+          <cell r="B3">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>"07</v>
+          </cell>
+          <cell r="B4">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>"08</v>
+          </cell>
+          <cell r="B5">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>"09</v>
+          </cell>
+          <cell r="B6">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>"10</v>
+          </cell>
+          <cell r="B7">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>"11</v>
+          </cell>
+          <cell r="B8">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>"12</v>
+          </cell>
+          <cell r="B9">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>"13</v>
+          </cell>
+          <cell r="B10">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>"14</v>
+          </cell>
+          <cell r="B11">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>"15</v>
+          </cell>
+          <cell r="B12">
+            <v>8</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Number of injuries</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>"05</v>
+          </cell>
+          <cell r="B2">
+            <v>893</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>"06</v>
+          </cell>
+          <cell r="B3">
+            <v>970</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>"07</v>
+          </cell>
+          <cell r="B4">
+            <v>929</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>"08</v>
+          </cell>
+          <cell r="B5">
+            <v>848</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>"09</v>
+          </cell>
+          <cell r="B6">
+            <v>979</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>"10</v>
+          </cell>
+          <cell r="B7">
+            <v>896</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>"11</v>
+          </cell>
+          <cell r="B8">
+            <v>757</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>"12</v>
+          </cell>
+          <cell r="B9">
+            <v>733</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>"13</v>
+          </cell>
+          <cell r="B10">
+            <v>662</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>"14</v>
+          </cell>
+          <cell r="B11">
+            <v>623</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>"15</v>
+          </cell>
+          <cell r="B12">
+            <v>652</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="fatal_cir"/>
+      <sheetName val="fixed_object"/>
+      <sheetName val="fatal_fixed_object"/>
+      <sheetName val="fatal_mv"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="fatal_safetydevice"/>
+      <sheetName val="fatal_safetydevice_driver"/>
+      <sheetName val="fatal_safetydevice_motorcycle"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>18 alcohol</v>
+          </cell>
+          <cell r="B2">
+            <v>24</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>4 speed</v>
+          </cell>
+          <cell r="B3">
+            <v>24</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>13 improper lane usage/change</v>
+          </cell>
+          <cell r="B4">
+            <v>19</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>17 Failed to Yield</v>
+          </cell>
+          <cell r="B5">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>22 None</v>
+          </cell>
+          <cell r="B6">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>19 Drugs</v>
+          </cell>
+          <cell r="B7">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>20 Physical impairment</v>
+          </cell>
+          <cell r="B8">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>5 Too fast for conditions</v>
+          </cell>
+          <cell r="B9">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>14 wrong side (one-way)</v>
+          </cell>
+          <cell r="B10">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>28 Overcorrected</v>
+          </cell>
+          <cell r="B11">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>21 Distracted/Inattentative</v>
+          </cell>
+          <cell r="B12">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>9 Following too close</v>
+          </cell>
+          <cell r="B13">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>U Uknown</v>
+          </cell>
+          <cell r="B14">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>1 Vehicle Defects</v>
+          </cell>
+          <cell r="B15">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>26 failed to yield</v>
+          </cell>
+          <cell r="B16">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>3 Improperly Stopped On Roadway</v>
+          </cell>
+          <cell r="B17">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>SpeedExceededLimit</v>
+          </cell>
+          <cell r="B28">
+            <v>37</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>Alcohol</v>
+          </cell>
+          <cell r="B29">
+            <v>36</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>None</v>
+          </cell>
+          <cell r="B30">
+            <v>28</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>ImproperLaneUsage/Change</v>
+          </cell>
+          <cell r="B31">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>Drugs</v>
+          </cell>
+          <cell r="B32">
+            <v>12</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>FailedtoYield</v>
+          </cell>
+          <cell r="B33">
+            <v>11</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="D2" t="str">
+            <v>4 SpeedExceededLimit</v>
+          </cell>
+          <cell r="E2">
+            <v>22</v>
+          </cell>
+          <cell r="G2" t="str">
+            <v>4 SpeedExceededLimit</v>
+          </cell>
+          <cell r="H2">
+            <v>27</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="D3" t="str">
+            <v>18 Alcohol</v>
+          </cell>
+          <cell r="E3">
+            <v>16</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>18 Alcohol</v>
+          </cell>
+          <cell r="H3">
+            <v>22</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="D4" t="str">
+            <v>13 ImproperLaneUsage/Change</v>
+          </cell>
+          <cell r="E4">
+            <v>15</v>
+          </cell>
+          <cell r="G4" t="str">
+            <v>13 ImproperLaneUsage/Change</v>
+          </cell>
+          <cell r="H4">
+            <v>17</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="D5" t="str">
+            <v>19 Drugs</v>
+          </cell>
+          <cell r="E5">
+            <v>5</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>19 Drugs</v>
+          </cell>
+          <cell r="H5">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="D6" t="str">
+            <v>20 PhysicalImpairment</v>
+          </cell>
+          <cell r="E6">
+            <v>3</v>
+          </cell>
+          <cell r="G6" t="str">
+            <v>20 PhysicalImpairment</v>
+          </cell>
+          <cell r="H6">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>5 TooFastforConditions</v>
+          </cell>
+          <cell r="E7">
+            <v>3</v>
+          </cell>
+          <cell r="G7" t="str">
+            <v>5 TooFastforConditions</v>
+          </cell>
+          <cell r="H7">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8" t="str">
+            <v>28 Overcorrected</v>
+          </cell>
+          <cell r="E8">
+            <v>2</v>
+          </cell>
+          <cell r="G8" t="str">
+            <v>28 Overcorrected</v>
+          </cell>
+          <cell r="H8">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="D9" t="str">
+            <v>1 VehicleDefects</v>
+          </cell>
+          <cell r="E9">
+            <v>1</v>
+          </cell>
+          <cell r="G9" t="str">
+            <v>1 VehicleDefects</v>
+          </cell>
+          <cell r="H9">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="G10" t="str">
+            <v>7 ViolationSignal/Sign</v>
+          </cell>
+          <cell r="H10">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="G11" t="str">
+            <v>6 ImproperPassing</v>
+          </cell>
+          <cell r="H11">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="G12" t="str">
+            <v>None</v>
+          </cell>
+          <cell r="H12">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>no of fatalities</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>2 no safety device used</v>
+          </cell>
+          <cell r="B2">
+            <v>36</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>5 shoulder and lap belt</v>
+          </cell>
+          <cell r="B3">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>1 vehicle not equipped with seat belt</v>
+          </cell>
+          <cell r="B4">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>7 helmet used</v>
+          </cell>
+          <cell r="B5">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v xml:space="preserve">U </v>
+          </cell>
+          <cell r="B6">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>8 helmet not used</v>
+          </cell>
+          <cell r="B7">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>13 other helmet</v>
+          </cell>
+          <cell r="B8">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="crashes_by_year"/>
       <sheetName val="injured_fatal_crashes_by_year"/>
       <sheetName val="persons_by_year"/>
@@ -3305,410 +4036,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="fatal_cir"/>
-      <sheetName val="fixed_object"/>
-      <sheetName val="fatal_fixed_object"/>
-      <sheetName val="fatal_mv"/>
-      <sheetName val="Sheet3"/>
-      <sheetName val="fatal_safetydevice"/>
-      <sheetName val="fatal_safetydevice_driver"/>
-      <sheetName val="fatal_safetydevice_motorcycle"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>18 alcohol</v>
-          </cell>
-          <cell r="B2">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>4 speed</v>
-          </cell>
-          <cell r="B3">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>13 improper lane usage/change</v>
-          </cell>
-          <cell r="B4">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>17 Failed to Yield</v>
-          </cell>
-          <cell r="B5">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>22 None</v>
-          </cell>
-          <cell r="B6">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>19 Drugs</v>
-          </cell>
-          <cell r="B7">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>20 Physical impairment</v>
-          </cell>
-          <cell r="B8">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>5 Too fast for conditions</v>
-          </cell>
-          <cell r="B9">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>14 wrong side (one-way)</v>
-          </cell>
-          <cell r="B10">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>28 Overcorrected</v>
-          </cell>
-          <cell r="B11">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>21 Distracted/Inattentative</v>
-          </cell>
-          <cell r="B12">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>9 Following too close</v>
-          </cell>
-          <cell r="B13">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>U Uknown</v>
-          </cell>
-          <cell r="B14">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>1 Vehicle Defects</v>
-          </cell>
-          <cell r="B15">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>26 failed to yield</v>
-          </cell>
-          <cell r="B16">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>3 Improperly Stopped On Roadway</v>
-          </cell>
-          <cell r="B17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>SpeedExceededLimit</v>
-          </cell>
-          <cell r="B28">
-            <v>37</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>Alcohol</v>
-          </cell>
-          <cell r="B29">
-            <v>36</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>None</v>
-          </cell>
-          <cell r="B30">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>ImproperLaneUsage/Change</v>
-          </cell>
-          <cell r="B31">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>Drugs</v>
-          </cell>
-          <cell r="B32">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>FailedtoYield</v>
-          </cell>
-          <cell r="B33">
-            <v>11</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="D2" t="str">
-            <v>4 SpeedExceededLimit</v>
-          </cell>
-          <cell r="E2">
-            <v>22</v>
-          </cell>
-          <cell r="G2" t="str">
-            <v>4 SpeedExceededLimit</v>
-          </cell>
-          <cell r="H2">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3" t="str">
-            <v>18 Alcohol</v>
-          </cell>
-          <cell r="E3">
-            <v>16</v>
-          </cell>
-          <cell r="G3" t="str">
-            <v>18 Alcohol</v>
-          </cell>
-          <cell r="H3">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>13 ImproperLaneUsage/Change</v>
-          </cell>
-          <cell r="E4">
-            <v>15</v>
-          </cell>
-          <cell r="G4" t="str">
-            <v>13 ImproperLaneUsage/Change</v>
-          </cell>
-          <cell r="H4">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>19 Drugs</v>
-          </cell>
-          <cell r="E5">
-            <v>5</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>19 Drugs</v>
-          </cell>
-          <cell r="H5">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>20 PhysicalImpairment</v>
-          </cell>
-          <cell r="E6">
-            <v>3</v>
-          </cell>
-          <cell r="G6" t="str">
-            <v>20 PhysicalImpairment</v>
-          </cell>
-          <cell r="H6">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>5 TooFastforConditions</v>
-          </cell>
-          <cell r="E7">
-            <v>3</v>
-          </cell>
-          <cell r="G7" t="str">
-            <v>5 TooFastforConditions</v>
-          </cell>
-          <cell r="H7">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>28 Overcorrected</v>
-          </cell>
-          <cell r="E8">
-            <v>2</v>
-          </cell>
-          <cell r="G8" t="str">
-            <v>28 Overcorrected</v>
-          </cell>
-          <cell r="H8">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9" t="str">
-            <v>1 VehicleDefects</v>
-          </cell>
-          <cell r="E9">
-            <v>1</v>
-          </cell>
-          <cell r="G9" t="str">
-            <v>1 VehicleDefects</v>
-          </cell>
-          <cell r="H9">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="G10" t="str">
-            <v>7 ViolationSignal/Sign</v>
-          </cell>
-          <cell r="H10">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="G11" t="str">
-            <v>6 ImproperPassing</v>
-          </cell>
-          <cell r="H11">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="G12" t="str">
-            <v>None</v>
-          </cell>
-          <cell r="H12">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>no of fatalities</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>2 no safety device used</v>
-          </cell>
-          <cell r="B2">
-            <v>36</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>5 shoulder and lap belt</v>
-          </cell>
-          <cell r="B3">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>1 vehicle not equipped with seat belt</v>
-          </cell>
-          <cell r="B4">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>7 helmet used</v>
-          </cell>
-          <cell r="B5">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v xml:space="preserve">U </v>
-          </cell>
-          <cell r="B6">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>8 helmet not used</v>
-          </cell>
-          <cell r="B7">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>13 other helmet</v>
-          </cell>
-          <cell r="B8">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3965,472 +4293,6 @@
         <row r="1">
           <cell r="B1" t="str">
             <v>no of crashes</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>20 Tree/Stump</v>
-          </cell>
-          <cell r="B2">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>29 Crub</v>
-          </cell>
-          <cell r="B3">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>43 Other Post/Pole/Support</v>
-          </cell>
-          <cell r="B4">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>21 Embankment/Driveway/Ground/Rock Bluff</v>
-          </cell>
-          <cell r="B5">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>23 Utility Pole</v>
-          </cell>
-          <cell r="B6">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>27 Highway Traffic Sign Post</v>
-          </cell>
-          <cell r="B7">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>42 Ditch</v>
-          </cell>
-          <cell r="B8">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>36 Other</v>
-          </cell>
-          <cell r="B9">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>33 Traffic Signal Support</v>
-          </cell>
-          <cell r="B10">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>24 Fence</v>
-          </cell>
-          <cell r="B11">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>31 Concrete Traffic Barrier</v>
-          </cell>
-          <cell r="B12">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>22 Guardrail Face</v>
-          </cell>
-          <cell r="B13">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>28 Bridge Pier/Abutment/Support</v>
-          </cell>
-          <cell r="B14">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>39 Guardrail End</v>
-          </cell>
-          <cell r="B15">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>26 Culvert</v>
-          </cell>
-          <cell r="B16">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>41 Overhead Sign Support</v>
-          </cell>
-          <cell r="B17">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Number of crashes"/>
-      <sheetName val="number of fatalities"/>
-      <sheetName val="number of injuries"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>no of 911 calls regarding collisions</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>no of STARS report</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>no of self-report</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>"05</v>
-          </cell>
-          <cell r="B2">
-            <v>6095</v>
-          </cell>
-          <cell r="C2">
-            <v>3469</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>"06</v>
-          </cell>
-          <cell r="B3">
-            <v>6009</v>
-          </cell>
-          <cell r="C3">
-            <v>3462</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>"07</v>
-          </cell>
-          <cell r="B4">
-            <v>6194</v>
-          </cell>
-          <cell r="C4">
-            <v>3158</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>"08</v>
-          </cell>
-          <cell r="B5">
-            <v>5659</v>
-          </cell>
-          <cell r="C5">
-            <v>2906</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>"09</v>
-          </cell>
-          <cell r="B6">
-            <v>5364</v>
-          </cell>
-          <cell r="C6">
-            <v>2780</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>"10</v>
-          </cell>
-          <cell r="B7">
-            <v>5738</v>
-          </cell>
-          <cell r="C7">
-            <v>1847</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>"11</v>
-          </cell>
-          <cell r="B8">
-            <v>5492</v>
-          </cell>
-          <cell r="C8">
-            <v>1585</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>"12</v>
-          </cell>
-          <cell r="B9">
-            <v>5401</v>
-          </cell>
-          <cell r="C9">
-            <v>1556</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>"13</v>
-          </cell>
-          <cell r="B10">
-            <v>5613</v>
-          </cell>
-          <cell r="C10">
-            <v>1561</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>"14</v>
-          </cell>
-          <cell r="B11">
-            <v>5838</v>
-          </cell>
-          <cell r="C11">
-            <v>1524</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>"15</v>
-          </cell>
-          <cell r="B12">
-            <v>5887</v>
-          </cell>
-          <cell r="C12">
-            <v>1380</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Number of fatalities</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>"05</v>
-          </cell>
-          <cell r="B2">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>"06</v>
-          </cell>
-          <cell r="B3">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>"07</v>
-          </cell>
-          <cell r="B4">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>"08</v>
-          </cell>
-          <cell r="B5">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>"09</v>
-          </cell>
-          <cell r="B6">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>"10</v>
-          </cell>
-          <cell r="B7">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>"11</v>
-          </cell>
-          <cell r="B8">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>"12</v>
-          </cell>
-          <cell r="B9">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>"13</v>
-          </cell>
-          <cell r="B10">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>"14</v>
-          </cell>
-          <cell r="B11">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>"15</v>
-          </cell>
-          <cell r="B12">
-            <v>8</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Number of injuries</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>"05</v>
-          </cell>
-          <cell r="B2">
-            <v>893</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>"06</v>
-          </cell>
-          <cell r="B3">
-            <v>970</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>"07</v>
-          </cell>
-          <cell r="B4">
-            <v>929</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>"08</v>
-          </cell>
-          <cell r="B5">
-            <v>848</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>"09</v>
-          </cell>
-          <cell r="B6">
-            <v>979</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>"10</v>
-          </cell>
-          <cell r="B7">
-            <v>896</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>"11</v>
-          </cell>
-          <cell r="B8">
-            <v>757</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>"12</v>
-          </cell>
-          <cell r="B9">
-            <v>733</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>"13</v>
-          </cell>
-          <cell r="B10">
-            <v>662</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>"14</v>
-          </cell>
-          <cell r="B11">
-            <v>623</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>"15</v>
-          </cell>
-          <cell r="B12">
-            <v>652</v>
           </cell>
         </row>
       </sheetData>
@@ -4763,8 +4625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4784,8 +4646,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
-      <c r="A2" s="1" t="s">
-        <v>150</v>
+      <c r="A2" s="1">
+        <v>2005</v>
       </c>
       <c r="B2" s="1">
         <v>6095</v>
@@ -4796,8 +4658,8 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="16">
-      <c r="A3" s="1" t="s">
-        <v>151</v>
+      <c r="A3" s="1">
+        <v>2006</v>
       </c>
       <c r="B3" s="1">
         <v>6009</v>
@@ -4808,8 +4670,8 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="16">
-      <c r="A4" s="1" t="s">
-        <v>152</v>
+      <c r="A4" s="1">
+        <v>2007</v>
       </c>
       <c r="B4" s="1">
         <v>6194</v>
@@ -4820,8 +4682,8 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="1" t="s">
-        <v>153</v>
+      <c r="A5" s="1">
+        <v>2008</v>
       </c>
       <c r="B5" s="1">
         <v>5659</v>
@@ -4832,8 +4694,8 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="1" t="s">
-        <v>154</v>
+      <c r="A6" s="1">
+        <v>2009</v>
       </c>
       <c r="B6" s="1">
         <v>5364</v>
@@ -4844,8 +4706,8 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="1" t="s">
-        <v>155</v>
+      <c r="A7" s="1">
+        <v>2010</v>
       </c>
       <c r="B7" s="1">
         <v>5738</v>
@@ -4856,8 +4718,8 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="16">
-      <c r="A8" s="1" t="s">
-        <v>156</v>
+      <c r="A8" s="1">
+        <v>2011</v>
       </c>
       <c r="B8" s="1">
         <v>5492</v>
@@ -4868,8 +4730,8 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="1" t="s">
-        <v>157</v>
+      <c r="A9" s="1">
+        <v>2012</v>
       </c>
       <c r="B9" s="1">
         <v>5401</v>
@@ -4880,8 +4742,8 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="1" t="s">
-        <v>158</v>
+      <c r="A10" s="1">
+        <v>2013</v>
       </c>
       <c r="B10" s="1">
         <v>5613</v>
@@ -4892,8 +4754,8 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="1" t="s">
-        <v>159</v>
+      <c r="A11" s="1">
+        <v>2014</v>
       </c>
       <c r="B11" s="1">
         <v>5838</v>
@@ -4904,8 +4766,8 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="16">
-      <c r="A12" s="1" t="s">
-        <v>160</v>
+      <c r="A12" s="1">
+        <v>2015</v>
       </c>
       <c r="B12" s="1">
         <v>5887</v>
@@ -4917,6 +4779,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6321,7 +6184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>